<commit_message>
More work on Mistakenly Resolved checks.
</commit_message>
<xml_diff>
--- a/OPID/Uploads/File2 11302017 to 02282018.xlsx
+++ b/OPID/Uploads/File2 11302017 to 02282018.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Apricot\OPID\MSMUploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42F90CEC-5215-48CA-B6A6-FCBAEFE266C7}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8C296A6-4519-4B95-89F8-758296D14A93}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21975" windowHeight="7125" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -9813,8 +9813,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B1:N1247"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="P12" sqref="P12"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="O68" sqref="O68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>